<commit_message>
Corrected and added constant and configuration files with new tile identification section (xlsx and yml)
</commit_message>
<xml_diff>
--- a/results/Finse_4432/Finse_4432.xlsx
+++ b/results/Finse_4432/Finse_4432.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\git\CryoGrid2020_22\results\Finse_4432\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joasc\Documents\Research\Modeling\CryoGrid\Model_versions &amp; runs\CryoGrid_OOP_JOASC\results\Finse_4432\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="129">
   <si>
     <t xml:space="preserve">    </t>
   </si>
@@ -408,6 +408,9 @@
   </si>
   <si>
     <t>GROUND_freeW_bucketW_seb</t>
+  </si>
+  <si>
+    <t>01.10.2014</t>
   </si>
 </sst>
 </file>
@@ -752,22 +755,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.85546875" customWidth="1"/>
-    <col min="2" max="2" width="50.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="41.81640625" customWidth="1"/>
+    <col min="2" max="2" width="50.1796875" customWidth="1"/>
+    <col min="3" max="3" width="16.26953125" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" customWidth="1"/>
+    <col min="5" max="5" width="17.453125" customWidth="1"/>
+    <col min="6" max="6" width="16.26953125" customWidth="1"/>
+    <col min="9" max="9" width="11.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>71</v>
       </c>
@@ -775,7 +778,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>88</v>
       </c>
@@ -783,7 +786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>74</v>
       </c>
@@ -794,7 +797,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -805,7 +808,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -819,17 +822,17 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>52</v>
       </c>
@@ -837,7 +840,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>60</v>
       </c>
@@ -845,7 +848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -853,18 +856,18 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="5">
-        <v>41913</v>
+      <c r="B15" s="5" t="s">
+        <v>128</v>
       </c>
       <c r="D15" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -872,7 +875,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -886,7 +889,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -900,7 +903,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -914,7 +917,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -925,7 +928,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>57</v>
       </c>
@@ -939,7 +942,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -953,7 +956,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -967,7 +970,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -981,17 +984,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>30</v>
       </c>
@@ -999,7 +1002,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>62</v>
       </c>
@@ -1007,7 +1010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>31</v>
       </c>
@@ -1018,7 +1021,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -1029,12 +1032,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>0</v>
       </c>
@@ -1045,7 +1048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>1</v>
       </c>
@@ -1056,7 +1059,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>3</v>
       </c>
@@ -1067,7 +1070,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>5</v>
       </c>
@@ -1078,7 +1081,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>50</v>
       </c>
@@ -1089,22 +1092,22 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>21</v>
       </c>
@@ -1115,7 +1118,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>61</v>
       </c>
@@ -1123,7 +1126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>26</v>
       </c>
@@ -1158,7 +1161,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>6</v>
       </c>
@@ -1184,12 +1187,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>0</v>
       </c>
@@ -1224,7 +1227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>8</v>
       </c>
@@ -1259,7 +1262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>12</v>
       </c>
@@ -1294,17 +1297,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>21</v>
       </c>
@@ -1312,7 +1315,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>63</v>
       </c>
@@ -1320,7 +1323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
         <v>26</v>
       </c>
@@ -1331,17 +1334,17 @@
         <v>94</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>0</v>
       </c>
@@ -1352,7 +1355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>8</v>
       </c>
@@ -1363,7 +1366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>10</v>
       </c>
@@ -1374,16 +1377,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>36</v>
       </c>
       <c r="B65" s="4"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B66" s="4"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>120</v>
       </c>
@@ -1392,7 +1395,7 @@
       </c>
       <c r="C67" s="8"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>95</v>
       </c>
@@ -1401,12 +1404,12 @@
       </c>
       <c r="C68" s="8"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>21</v>
       </c>
@@ -1417,7 +1420,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>65</v>
       </c>
@@ -1425,7 +1428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
         <v>26</v>
       </c>
@@ -1433,7 +1436,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>6</v>
       </c>
@@ -1441,12 +1444,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>0</v>
       </c>
@@ -1454,7 +1457,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>8</v>
       </c>
@@ -1462,7 +1465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>10</v>
       </c>
@@ -1470,7 +1473,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>100</v>
       </c>
@@ -1478,7 +1481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>5000</v>
       </c>
@@ -1486,22 +1489,22 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="2" t="s">
         <v>15</v>
       </c>
@@ -1509,7 +1512,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="2" t="s">
         <v>108</v>
       </c>
@@ -1517,10 +1520,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B90" s="6"/>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B91" s="6" t="s">
         <v>17</v>
       </c>
@@ -1531,7 +1534,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>1</v>
       </c>
@@ -1548,7 +1551,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>2</v>
       </c>
@@ -1565,7 +1568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>3</v>
       </c>
@@ -1582,7 +1585,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>92</v>
       </c>
@@ -1591,7 +1594,7 @@
       </c>
       <c r="C95" s="6"/>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>89</v>
       </c>
@@ -1608,7 +1611,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>0</v>
       </c>
@@ -1622,7 +1625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>67</v>
       </c>
@@ -1639,7 +1642,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>68</v>
       </c>
@@ -1656,11 +1659,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B100" s="6"/>
       <c r="C100" s="6"/>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>86</v>
       </c>
@@ -1672,26 +1675,26 @@
         <v>87</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>44</v>
       </c>
       <c r="B102" s="6"/>
       <c r="C102" s="6"/>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B103" s="6"/>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B104" s="6"/>
       <c r="C104" s="6"/>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="2" t="s">
         <v>15</v>
       </c>
@@ -1700,7 +1703,7 @@
       </c>
       <c r="C106" s="6"/>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
         <v>122</v>
       </c>
@@ -1709,11 +1712,11 @@
       </c>
       <c r="C107" s="6"/>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B108" s="6"/>
       <c r="C108" s="6"/>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B109" s="6" t="s">
         <v>17</v>
       </c>
@@ -1724,7 +1727,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>1</v>
       </c>
@@ -1741,7 +1744,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>2</v>
       </c>
@@ -1758,7 +1761,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>3</v>
       </c>
@@ -1775,7 +1778,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>92</v>
       </c>
@@ -1784,7 +1787,7 @@
       </c>
       <c r="C113" s="6"/>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>89</v>
       </c>
@@ -1801,11 +1804,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B115" s="6"/>
       <c r="C115" s="6"/>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>97</v>
       </c>
@@ -1814,7 +1817,7 @@
       </c>
       <c r="C116" s="6"/>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>98</v>
       </c>
@@ -1823,7 +1826,7 @@
       </c>
       <c r="C117" s="6"/>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>99</v>
       </c>
@@ -1832,7 +1835,7 @@
       </c>
       <c r="C118" s="6"/>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>100</v>
       </c>
@@ -1841,11 +1844,11 @@
       </c>
       <c r="C119" s="6"/>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B120" s="6"/>
       <c r="C120" s="6"/>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>114</v>
       </c>
@@ -1854,7 +1857,7 @@
       </c>
       <c r="C121" s="6"/>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>115</v>
       </c>
@@ -1863,7 +1866,7 @@
       </c>
       <c r="C122" s="6"/>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>116</v>
       </c>
@@ -1877,7 +1880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>118</v>
       </c>
@@ -1894,7 +1897,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>117</v>
       </c>
@@ -1911,7 +1914,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>119</v>
       </c>
@@ -1920,7 +1923,7 @@
       </c>
       <c r="C126" s="6"/>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>0</v>
       </c>
@@ -1932,7 +1935,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>67</v>
       </c>
@@ -1941,7 +1944,7 @@
       </c>
       <c r="C128" s="6"/>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>68</v>
       </c>
@@ -1950,10 +1953,10 @@
       </c>
       <c r="C129" s="6"/>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B130" s="6"/>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>86</v>
       </c>
@@ -1962,14 +1965,14 @@
       </c>
       <c r="C131" s="6"/>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>44</v>
       </c>
       <c r="B132" s="6"/>
       <c r="C132" s="6"/>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
         <v>25</v>
       </c>
@@ -1980,7 +1983,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="2" t="s">
         <v>15</v>
       </c>
@@ -1989,7 +1992,7 @@
       </c>
       <c r="C135" s="6"/>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="2" t="s">
         <v>123</v>
       </c>
@@ -1998,11 +2001,11 @@
       </c>
       <c r="C136" s="6"/>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B137" s="6"/>
       <c r="C137" s="6"/>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B138" s="6" t="s">
         <v>17</v>
       </c>
@@ -2016,7 +2019,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>109</v>
       </c>
@@ -2033,7 +2036,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>111</v>
       </c>
@@ -2042,7 +2045,7 @@
       </c>
       <c r="C140" s="6"/>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>110</v>
       </c>
@@ -2054,7 +2057,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>2</v>
       </c>
@@ -2063,7 +2066,7 @@
       </c>
       <c r="C142" s="6"/>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>3</v>
       </c>
@@ -2072,7 +2075,7 @@
       </c>
       <c r="C143" s="6"/>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>92</v>
       </c>
@@ -2081,7 +2084,7 @@
       </c>
       <c r="C144" s="6"/>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>112</v>
       </c>
@@ -2098,7 +2101,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>49</v>
       </c>
@@ -2115,7 +2118,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>97</v>
       </c>
@@ -2124,7 +2127,7 @@
       </c>
       <c r="C147" s="6"/>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>107</v>
       </c>
@@ -2133,7 +2136,7 @@
       </c>
       <c r="C148" s="6"/>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>67</v>
       </c>
@@ -2142,7 +2145,7 @@
       </c>
       <c r="C149" s="6"/>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>68</v>
       </c>
@@ -2151,26 +2154,26 @@
       </c>
       <c r="C150" s="6"/>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B151" s="6"/>
       <c r="C151" s="6"/>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>44</v>
       </c>
       <c r="B152" s="6"/>
       <c r="C152" s="6"/>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C153" s="6"/>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" s="2" t="s">
         <v>15</v>
       </c>
@@ -2178,7 +2181,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" s="2" t="s">
         <v>105</v>
       </c>
@@ -2186,10 +2189,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B157" s="6"/>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B158" s="6" t="s">
         <v>17</v>
       </c>
@@ -2200,7 +2203,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>1</v>
       </c>
@@ -2217,7 +2220,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>101</v>
       </c>
@@ -2234,7 +2237,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>2</v>
       </c>
@@ -2251,7 +2254,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>3</v>
       </c>
@@ -2268,7 +2271,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>92</v>
       </c>
@@ -2277,7 +2280,7 @@
       </c>
       <c r="C163" s="6"/>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>89</v>
       </c>
@@ -2294,7 +2297,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>106</v>
       </c>
@@ -2308,7 +2311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>49</v>
       </c>
@@ -2317,11 +2320,11 @@
       </c>
       <c r="C166" s="6"/>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B167" s="6"/>
       <c r="C167" s="6"/>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>107</v>
       </c>
@@ -2330,7 +2333,7 @@
       </c>
       <c r="C168" s="6"/>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>67</v>
       </c>
@@ -2347,7 +2350,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>68</v>
       </c>
@@ -2364,25 +2367,25 @@
         <v>14</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>44</v>
       </c>
       <c r="B171" s="6"/>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B172" s="6"/>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B173" s="6"/>
       <c r="C173" s="6"/>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" s="2" t="s">
         <v>15</v>
       </c>
@@ -2391,10 +2394,10 @@
       </c>
       <c r="C175" s="6"/>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B176" s="6"/>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" s="2" t="s">
         <v>15</v>
       </c>
@@ -2402,7 +2405,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" s="2" t="s">
         <v>126</v>
       </c>
@@ -2410,7 +2413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B181" t="s">
         <v>17</v>
       </c>
@@ -2421,7 +2424,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>1</v>
       </c>
@@ -2438,7 +2441,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>2</v>
       </c>
@@ -2455,7 +2458,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>3</v>
       </c>
@@ -2472,7 +2475,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>89</v>
       </c>
@@ -2489,7 +2492,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>0</v>
       </c>
@@ -2503,7 +2506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>67</v>
       </c>
@@ -2520,7 +2523,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>68</v>
       </c>
@@ -2537,7 +2540,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>86</v>
       </c>
@@ -2548,7 +2551,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>97</v>
       </c>
@@ -2556,7 +2559,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>98</v>
       </c>
@@ -2564,7 +2567,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>99</v>
       </c>
@@ -2572,7 +2575,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>100</v>
       </c>
@@ -2580,20 +2583,20 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A199" s="2"/>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A200" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A201" s="2" t="s">
         <v>15</v>
       </c>
@@ -2602,10 +2605,10 @@
       </c>
       <c r="C201" s="6"/>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B202" s="6"/>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A204" s="2" t="s">
         <v>15</v>
       </c>
@@ -2613,7 +2616,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A205" s="2" t="s">
         <v>127</v>
       </c>
@@ -2621,7 +2624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B207" t="s">
         <v>17</v>
       </c>
@@ -2632,7 +2635,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>1</v>
       </c>
@@ -2649,7 +2652,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>2</v>
       </c>
@@ -2666,7 +2669,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>3</v>
       </c>
@@ -2683,7 +2686,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>89</v>
       </c>
@@ -2700,7 +2703,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>0</v>
       </c>
@@ -2714,7 +2717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>67</v>
       </c>
@@ -2731,7 +2734,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>68</v>
       </c>
@@ -2748,7 +2751,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>86</v>
       </c>
@@ -2759,7 +2762,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>97</v>
       </c>
@@ -2767,7 +2770,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>98</v>
       </c>
@@ -2775,7 +2778,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>99</v>
       </c>
@@ -2783,7 +2786,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>100</v>
       </c>
@@ -2791,158 +2794,158 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A225" s="2"/>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B226" s="6"/>
       <c r="C226" s="6"/>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B227" s="6"/>
       <c r="C227" s="6"/>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B228" s="6"/>
       <c r="C228" s="6"/>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B229" s="6"/>
       <c r="C229" s="6"/>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B230" s="6"/>
       <c r="C230" s="6"/>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B231" s="6"/>
       <c r="C231" s="6"/>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B232" s="6"/>
       <c r="C232" s="6"/>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B233" s="6"/>
       <c r="C233" s="6"/>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B234" s="6"/>
       <c r="C234" s="6"/>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B235" s="6"/>
       <c r="C235" s="6"/>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B236" s="6"/>
       <c r="C236" s="6"/>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B237" s="6"/>
       <c r="C237" s="6"/>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B238" s="6"/>
       <c r="C238" s="6"/>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B239" s="6"/>
       <c r="C239" s="6"/>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B240" s="6"/>
       <c r="C240" s="6"/>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B241" s="6"/>
       <c r="C241" s="6"/>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B242" s="6"/>
       <c r="C242" s="6"/>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B243" s="6"/>
       <c r="C243" s="6"/>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B246" s="6"/>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B247" s="6"/>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A248" s="1"/>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A249" s="2"/>
       <c r="B249" s="7"/>
       <c r="C249" s="6"/>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A250" s="2"/>
       <c r="B250" s="7"/>
       <c r="C250" s="6"/>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B251" s="6"/>
       <c r="C251" s="6"/>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B252" s="6"/>
       <c r="C252" s="6"/>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B253" s="6"/>
       <c r="C253" s="6"/>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B254" s="6"/>
       <c r="C254" s="6"/>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B255" s="6"/>
       <c r="C255" s="6"/>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B256" s="6"/>
       <c r="C256" s="6"/>
     </row>
-    <row r="257" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="257" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B257" s="6"/>
       <c r="C257" s="6"/>
     </row>
-    <row r="258" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="258" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B258" s="6"/>
       <c r="C258" s="6"/>
     </row>
-    <row r="259" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="259" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B259" s="6"/>
       <c r="C259" s="6"/>
     </row>
-    <row r="260" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="260" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B260" s="6"/>
       <c r="C260" s="6"/>
     </row>
-    <row r="261" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="261" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B261" s="6"/>
       <c r="C261" s="6"/>
     </row>
-    <row r="262" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="262" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B262" s="6"/>
       <c r="C262" s="6"/>
     </row>
-    <row r="263" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="263" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B263" s="6"/>
       <c r="C263" s="6"/>
     </row>
-    <row r="264" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="264" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C264" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Classes and input files used in "run_CG_Finse", "run_CG_Finse_YAML" and "run_CG_Suossjavri" updated so these model setups are all runnable.
</commit_message>
<xml_diff>
--- a/results/Finse_4432/Finse_4432.xlsx
+++ b/results/Finse_4432/Finse_4432.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\work\CryoGrid2020_27\results\Finse_4432\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\thin\02_Code\Matlab\CryoGRID\202008_CryoGrid_NewOOP_GIT - CURRENT_THIN\results\Finse_4432\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="151">
   <si>
     <t xml:space="preserve">    </t>
   </si>
@@ -474,6 +474,9 @@
   </si>
   <si>
     <t>Xice</t>
+  </si>
+  <si>
+    <t>01.10.2014</t>
   </si>
 </sst>
 </file>
@@ -818,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G278"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="G67" sqref="G67"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,8 +1084,8 @@
       <c r="A30" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="5">
-        <v>41913</v>
+      <c r="B30" s="5" t="s">
+        <v>150</v>
       </c>
       <c r="D30" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
Finse_4432 YAML and EXCEL parameter files updated to include list of lateral interactions. List is read and parsed by PARAMETER_PROVIDERs, which now have a property "tile_info" containing the parsed tile_identification information. TILE_BUILDER updated to query the new property.
</commit_message>
<xml_diff>
--- a/results/Finse_4432/Finse_4432.xlsx
+++ b/results/Finse_4432/Finse_4432.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="155">
   <si>
     <t xml:space="preserve">    </t>
   </si>
@@ -477,6 +477,18 @@
   </si>
   <si>
     <t>01.10.2014</t>
+  </si>
+  <si>
+    <t>LIST</t>
+  </si>
+  <si>
+    <t>END</t>
+  </si>
+  <si>
+    <t>LAT_WATER_RESERVOIR</t>
+  </si>
+  <si>
+    <t>lateral_interactions</t>
   </si>
 </sst>
 </file>
@@ -819,18 +831,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G278"/>
+  <dimension ref="A1:G279"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.85546875" customWidth="1"/>
-    <col min="2" max="2" width="50.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="2" max="4" width="23.140625" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" customWidth="1"/>
     <col min="6" max="6" width="16.28515625" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" customWidth="1"/>
@@ -987,446 +997,437 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C14" t="s">
+        <v>153</v>
+      </c>
+      <c r="D14" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-    </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="A17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>71</v>
-      </c>
-      <c r="B19">
-        <v>0.25</v>
-      </c>
-      <c r="C19" t="s">
-        <v>74</v>
+      <c r="B19" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>72</v>
-      </c>
-      <c r="B20" t="s">
-        <v>75</v>
+        <v>71</v>
+      </c>
+      <c r="B20">
+        <v>0.25</v>
       </c>
       <c r="C20" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>73</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
+        <v>72</v>
+      </c>
+      <c r="B21" t="s">
+        <v>75</v>
       </c>
       <c r="C21" t="s">
-        <v>77</v>
-      </c>
-      <c r="D21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>51</v>
-      </c>
-      <c r="B29" t="s">
-        <v>148</v>
+      <c r="B28" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>55</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="D30" t="s">
-        <v>67</v>
+        <v>51</v>
+      </c>
+      <c r="B30" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>150</v>
       </c>
       <c r="D31" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>52</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="D32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B33">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C33" t="s">
         <v>5</v>
       </c>
       <c r="D33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="B34">
-        <v>61</v>
+        <v>0.5</v>
       </c>
       <c r="C34" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B35">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="C35" t="s">
         <v>38</v>
       </c>
+      <c r="D35" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="B36">
-        <v>1222</v>
+        <v>12</v>
       </c>
       <c r="C36" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="B37">
-        <v>100</v>
+        <v>1222</v>
       </c>
       <c r="C37" t="s">
         <v>6</v>
       </c>
       <c r="D37" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="B38">
-        <v>0.05</v>
+        <v>100</v>
       </c>
       <c r="C38" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D38" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="B39">
-        <v>2</v>
+        <v>0.05</v>
       </c>
       <c r="C39" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D39" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B44" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+      <c r="B45" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B47" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C47" s="3" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>6</v>
-      </c>
-      <c r="B47" t="s">
-        <v>6</v>
-      </c>
-      <c r="C47" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>0</v>
-      </c>
-      <c r="B49">
-        <v>0.05</v>
-      </c>
-      <c r="C49">
-        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B50">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="C50">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51">
+        <v>0.1</v>
+      </c>
+      <c r="C51">
         <v>3</v>
-      </c>
-      <c r="B51">
-        <v>0.2</v>
-      </c>
-      <c r="C51">
-        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
+        <v>3</v>
+      </c>
+      <c r="B52">
+        <v>0.2</v>
+      </c>
+      <c r="C52">
         <v>5</v>
-      </c>
-      <c r="B52">
-        <v>0.5</v>
-      </c>
-      <c r="C52">
-        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
+        <v>5</v>
+      </c>
+      <c r="B53">
+        <v>0.5</v>
+      </c>
+      <c r="C53">
         <v>50</v>
       </c>
-      <c r="B53">
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>50</v>
+      </c>
+      <c r="B54">
         <v>10</v>
       </c>
-      <c r="C53">
+      <c r="C54">
         <v>100</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D58" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D59" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B59" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
+      <c r="B60" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B62" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C62" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="D62" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E61" s="3" t="s">
+      <c r="E62" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F61" s="3" t="s">
+      <c r="F62" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G61" s="3" t="s">
+      <c r="G62" s="3" t="s">
         <v>149</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>6</v>
-      </c>
-      <c r="B62" t="s">
-        <v>5</v>
-      </c>
-      <c r="C62" t="s">
-        <v>5</v>
-      </c>
-      <c r="D62" t="s">
-        <v>5</v>
-      </c>
-      <c r="E62" t="s">
-        <v>5</v>
-      </c>
-      <c r="F62" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>6</v>
+      </c>
+      <c r="B63" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" t="s">
+        <v>5</v>
+      </c>
+      <c r="E63" t="s">
+        <v>5</v>
+      </c>
+      <c r="F63" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>0</v>
-      </c>
-      <c r="B64">
-        <v>0.2</v>
-      </c>
-      <c r="C64">
-        <v>0.5</v>
-      </c>
-      <c r="D64">
-        <v>0</v>
-      </c>
-      <c r="E64">
-        <v>0.3</v>
-      </c>
-      <c r="F64">
-        <v>1</v>
-      </c>
-      <c r="G64">
-        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B65">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="C65">
         <v>0.5</v>
@@ -1438,7 +1439,7 @@
         <v>0.3</v>
       </c>
       <c r="F65">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -1446,7 +1447,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B66">
         <v>0.5</v>
@@ -1461,533 +1462,547 @@
         <v>0.3</v>
       </c>
       <c r="F66">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G66">
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>35</v>
+      <c r="A67">
+        <v>12</v>
+      </c>
+      <c r="B67">
+        <v>0.5</v>
+      </c>
+      <c r="C67">
+        <v>0.5</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>0.3</v>
+      </c>
+      <c r="F67">
+        <v>1</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B72" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
+      <c r="B73" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B75" t="s">
         <v>90</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C75" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>0</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C77">
-        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78">
+        <v>0</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79">
         <v>10</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B79" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="C79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>35</v>
       </c>
-      <c r="B79" s="4"/>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B80" s="4"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>116</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C81" s="8"/>
+      <c r="B81" s="4"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>92</v>
-      </c>
-      <c r="B82" s="4">
-        <v>1</v>
+        <v>116</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>118</v>
       </c>
       <c r="C82" s="8"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>92</v>
+      </c>
+      <c r="B83" s="4">
+        <v>1</v>
+      </c>
+      <c r="C83" s="8"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E86" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E87" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B87" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="3" t="s">
+      <c r="B88" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B90" s="3" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>6</v>
-      </c>
-      <c r="B90" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>6</v>
+      </c>
+      <c r="B91" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92">
-        <v>0</v>
-      </c>
-      <c r="B92">
-        <v>5</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B93">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B94">
-        <v>-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="B95">
-        <v>1</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
+        <v>100</v>
+      </c>
+      <c r="B96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97">
         <v>5000</v>
       </c>
-      <c r="B96">
+      <c r="B97">
         <v>20</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B102" s="7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B103" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B104" s="6"/>
+      <c r="B104" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B105" s="6" t="s">
+      <c r="B105" s="6"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B106" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C105" s="6" t="s">
+      <c r="C106" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D105" t="s">
+      <c r="D106" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>1</v>
-      </c>
-      <c r="B106" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="C106" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="D106" t="s">
-        <v>5</v>
-      </c>
-      <c r="E106" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B107" s="6">
-        <v>0.99</v>
+        <v>0.15</v>
       </c>
       <c r="C107" s="6">
-        <v>0.99</v>
+        <v>0.15</v>
       </c>
       <c r="D107" t="s">
         <v>5</v>
       </c>
       <c r="E107" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B108" s="6">
-        <v>1E-3</v>
+        <v>0.99</v>
       </c>
       <c r="C108" s="6">
-        <v>1E-3</v>
+        <v>0.99</v>
       </c>
       <c r="D108" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E108" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>89</v>
+        <v>3</v>
       </c>
       <c r="B109" s="6">
-        <v>100</v>
-      </c>
-      <c r="C109" s="6"/>
+        <v>1E-3</v>
+      </c>
+      <c r="C109" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="D109" t="s">
+        <v>6</v>
+      </c>
+      <c r="E109" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B110" s="6">
-        <v>1</v>
-      </c>
-      <c r="C110" s="6">
-        <v>1</v>
-      </c>
-      <c r="D110" t="s">
-        <v>87</v>
-      </c>
-      <c r="E110" t="s">
-        <v>88</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C110" s="6"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>0</v>
-      </c>
-      <c r="B111" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C111" s="6" t="s">
-        <v>0</v>
+        <v>86</v>
+      </c>
+      <c r="B111" s="6">
+        <v>1</v>
+      </c>
+      <c r="C111" s="6">
+        <v>1</v>
+      </c>
+      <c r="D111" t="s">
+        <v>87</v>
       </c>
       <c r="E111" t="s">
-        <v>0</v>
+        <v>88</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>64</v>
-      </c>
-      <c r="B112" s="6">
-        <v>3600</v>
-      </c>
-      <c r="C112" s="6">
-        <v>3600</v>
-      </c>
-      <c r="D112" t="s">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="B112" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C112" s="6" t="s">
+        <v>0</v>
       </c>
       <c r="E112" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
+        <v>64</v>
+      </c>
+      <c r="B113" s="6">
+        <v>3600</v>
+      </c>
+      <c r="C113" s="6">
+        <v>3600</v>
+      </c>
+      <c r="D113" t="s">
+        <v>7</v>
+      </c>
+      <c r="E113" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>65</v>
       </c>
-      <c r="B113" s="6">
+      <c r="B114" s="6">
         <v>50000</v>
       </c>
-      <c r="C113" s="6">
+      <c r="C114" s="6">
         <v>50000</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D114" t="s">
         <v>8</v>
       </c>
-      <c r="E113" t="s">
+      <c r="E114" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B114" s="6"/>
-      <c r="C114" s="6"/>
-    </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>83</v>
-      </c>
-      <c r="B115" s="6">
-        <v>3</v>
-      </c>
+      <c r="B115" s="6"/>
       <c r="C115" s="6"/>
-      <c r="E115" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
+        <v>83</v>
+      </c>
+      <c r="B116" s="6">
+        <v>3</v>
+      </c>
+      <c r="C116" s="6"/>
+      <c r="E116" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>43</v>
       </c>
-      <c r="B116" s="6"/>
-      <c r="C116" s="6"/>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B117" s="6"/>
+      <c r="C117" s="6"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B118" s="6"/>
-      <c r="C118" s="6"/>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
+      <c r="B119" s="6"/>
+      <c r="C119" s="6"/>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A120" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B120" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C120" s="6"/>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B121" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C121" s="6"/>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B121" s="7">
-        <v>1</v>
-      </c>
-      <c r="C121" s="6"/>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B122" s="6"/>
+      <c r="B122" s="7">
+        <v>1</v>
+      </c>
       <c r="C122" s="6"/>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B123" s="6" t="s">
+      <c r="B123" s="6"/>
+      <c r="C123" s="6"/>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B124" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C123" s="6" t="s">
+      <c r="C124" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D123" t="s">
+      <c r="D124" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>1</v>
-      </c>
-      <c r="B124" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="C124" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="D124" t="s">
-        <v>5</v>
-      </c>
-      <c r="E124" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B125" s="6">
-        <v>0.99</v>
+        <v>0.15</v>
       </c>
       <c r="C125" s="6">
-        <v>0.99</v>
+        <v>0.15</v>
       </c>
       <c r="D125" t="s">
         <v>5</v>
       </c>
       <c r="E125" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B126" s="6">
-        <v>1E-3</v>
+        <v>0.99</v>
       </c>
       <c r="C126" s="6">
-        <v>1E-3</v>
+        <v>0.99</v>
       </c>
       <c r="D126" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E126" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>89</v>
+        <v>3</v>
       </c>
       <c r="B127" s="6">
-        <v>100</v>
-      </c>
-      <c r="C127" s="6"/>
+        <v>1E-3</v>
+      </c>
+      <c r="C127" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="D127" t="s">
+        <v>6</v>
+      </c>
+      <c r="E127" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
+        <v>89</v>
+      </c>
+      <c r="B128" s="6">
+        <v>100</v>
+      </c>
+      <c r="C128" s="6"/>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
         <v>86</v>
       </c>
-      <c r="B128" s="6">
-        <v>1</v>
-      </c>
-      <c r="C128" s="6">
-        <v>1</v>
-      </c>
-      <c r="D128" t="s">
+      <c r="B129" s="6">
+        <v>1</v>
+      </c>
+      <c r="C129" s="6">
+        <v>1</v>
+      </c>
+      <c r="D129" t="s">
         <v>87</v>
       </c>
-      <c r="E128" t="s">
+      <c r="E129" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B129" s="6"/>
-      <c r="C129" s="6"/>
-    </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>93</v>
-      </c>
-      <c r="B130" s="9">
-        <v>1.0000000000000001E-5</v>
-      </c>
+      <c r="B130" s="6"/>
       <c r="C130" s="6"/>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>94</v>
-      </c>
-      <c r="B131">
-        <v>0.4</v>
+        <v>93</v>
+      </c>
+      <c r="B131" s="9">
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="C131" s="6"/>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B132">
         <v>0.4</v>
@@ -1996,29 +2011,29 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
+        <v>95</v>
+      </c>
+      <c r="B133">
+        <v>0.4</v>
+      </c>
+      <c r="C133" s="6"/>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
         <v>96</v>
       </c>
-      <c r="B133">
+      <c r="B134">
         <v>0.5</v>
       </c>
-      <c r="C133" s="6"/>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B134" s="6"/>
       <c r="C134" s="6"/>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>110</v>
-      </c>
-      <c r="B135" s="6">
-        <v>1000</v>
-      </c>
+      <c r="B135" s="6"/>
       <c r="C135" s="6"/>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B136" s="6">
         <v>1000</v>
@@ -2027,708 +2042,709 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B137" s="6">
-        <v>-30</v>
-      </c>
-      <c r="C137" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E137" t="s">
-        <v>0</v>
-      </c>
+        <v>1000</v>
+      </c>
+      <c r="C137" s="6"/>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B138" s="6">
-        <v>0.05</v>
-      </c>
-      <c r="C138" s="6">
-        <v>3600</v>
-      </c>
-      <c r="D138" t="s">
-        <v>7</v>
+        <v>-30</v>
+      </c>
+      <c r="C138" s="6" t="s">
+        <v>0</v>
       </c>
       <c r="E138" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B139" s="6">
-        <v>0.95</v>
+        <v>0.05</v>
       </c>
       <c r="C139" s="6">
-        <v>50000</v>
+        <v>3600</v>
       </c>
       <c r="D139" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E139" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B140" s="6">
-        <v>0.05</v>
-      </c>
-      <c r="C140" s="6"/>
+        <v>0.95</v>
+      </c>
+      <c r="C140" s="6">
+        <v>50000</v>
+      </c>
+      <c r="D140" t="s">
+        <v>8</v>
+      </c>
+      <c r="E140" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>0</v>
-      </c>
-      <c r="B141" s="6" t="s">
-        <v>0</v>
+        <v>115</v>
+      </c>
+      <c r="B141" s="6">
+        <v>0.05</v>
       </c>
       <c r="C141" s="6"/>
-      <c r="E141" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>64</v>
-      </c>
-      <c r="B142" s="6">
-        <v>3600</v>
+        <v>0</v>
+      </c>
+      <c r="B142" s="6" t="s">
+        <v>0</v>
       </c>
       <c r="C142" s="6"/>
+      <c r="E142" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
+        <v>64</v>
+      </c>
+      <c r="B143" s="6">
+        <v>3600</v>
+      </c>
+      <c r="C143" s="6"/>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
         <v>65</v>
       </c>
-      <c r="B143" s="6">
+      <c r="B144" s="6">
         <v>50000</v>
       </c>
-      <c r="C143" s="6"/>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B144" s="6"/>
+      <c r="C144" s="6"/>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>83</v>
-      </c>
-      <c r="B145" s="6">
-        <v>3</v>
-      </c>
-      <c r="C145" s="6"/>
+      <c r="B145" s="6"/>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
+        <v>83</v>
+      </c>
+      <c r="B146" s="6">
+        <v>3</v>
+      </c>
+      <c r="C146" s="6"/>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
         <v>43</v>
       </c>
-      <c r="B146" s="6"/>
-      <c r="C146" s="6"/>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A148" s="1" t="s">
+      <c r="B147" s="6"/>
+      <c r="C147" s="6"/>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C148" s="6" t="s">
+      <c r="C149" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D148" t="s">
+      <c r="D149" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A149" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B149" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C149" s="6"/>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B150" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C150" s="6"/>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B150" s="7">
-        <v>1</v>
-      </c>
-      <c r="C150" s="6"/>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B151" s="6"/>
+      <c r="B151" s="7">
+        <v>1</v>
+      </c>
       <c r="C151" s="6"/>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B152" s="6" t="s">
+      <c r="B152" s="6"/>
+      <c r="C152" s="6"/>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B153" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C152" s="6">
+      <c r="C153" s="6">
         <v>0.99</v>
       </c>
-      <c r="D152" t="s">
+      <c r="D153" t="s">
         <v>5</v>
       </c>
-      <c r="E152" t="s">
+      <c r="E153" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>105</v>
-      </c>
-      <c r="B153" s="6">
-        <v>0</v>
-      </c>
-      <c r="C153" s="6">
-        <v>1E-3</v>
-      </c>
-      <c r="D153" t="s">
-        <v>6</v>
-      </c>
-      <c r="E153" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B154" s="6">
-        <v>0.71</v>
-      </c>
-      <c r="C154" s="6"/>
+        <v>0</v>
+      </c>
+      <c r="C154" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="D154" t="s">
+        <v>6</v>
+      </c>
+      <c r="E154" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B155" s="6">
-        <v>0.21</v>
+        <v>0.71</v>
       </c>
       <c r="C155" s="6"/>
-      <c r="D155" t="s">
-        <v>109</v>
-      </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>2</v>
+        <v>106</v>
       </c>
       <c r="B156" s="6">
-        <v>0.99</v>
+        <v>0.21</v>
       </c>
       <c r="C156" s="6"/>
+      <c r="D156" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B157" s="6">
-        <v>1E-3</v>
+        <v>0.99</v>
       </c>
       <c r="C157" s="6"/>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>89</v>
+        <v>3</v>
       </c>
       <c r="B158" s="6">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="C158" s="6"/>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="B159" s="6">
-        <v>48</v>
-      </c>
-      <c r="C159" s="6">
-        <v>3600</v>
-      </c>
-      <c r="D159" t="s">
-        <v>7</v>
-      </c>
-      <c r="E159" t="s">
-        <v>13</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C159" s="6"/>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
+        <v>108</v>
+      </c>
+      <c r="B160" s="6">
         <v>48</v>
       </c>
-      <c r="B160" s="6">
-        <v>0.05</v>
-      </c>
       <c r="C160" s="6">
-        <v>50000</v>
+        <v>3600</v>
       </c>
       <c r="D160" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E160" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>93</v>
-      </c>
-      <c r="B161" s="9">
-        <v>1E-4</v>
-      </c>
-      <c r="C161" s="6"/>
+        <v>48</v>
+      </c>
+      <c r="B161" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="C161" s="6">
+        <v>50000</v>
+      </c>
+      <c r="D161" t="s">
+        <v>8</v>
+      </c>
+      <c r="E161" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>103</v>
-      </c>
-      <c r="B162" s="6">
-        <v>0.02</v>
+        <v>93</v>
+      </c>
+      <c r="B162" s="9">
+        <v>1E-4</v>
       </c>
       <c r="C162" s="6"/>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="B163" s="6">
-        <v>3600</v>
+        <v>0.02</v>
       </c>
       <c r="C163" s="6"/>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
+        <v>64</v>
+      </c>
+      <c r="B164" s="6">
+        <v>3600</v>
+      </c>
+      <c r="C164" s="6"/>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
         <v>65</v>
       </c>
-      <c r="B164" s="6">
+      <c r="B165" s="6">
         <v>50000</v>
       </c>
-      <c r="C164" s="6"/>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B165" s="6"/>
       <c r="C165" s="6"/>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>43</v>
-      </c>
       <c r="B166" s="6"/>
       <c r="C166" s="6"/>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>43</v>
+      </c>
+      <c r="B167" s="6"/>
       <c r="C167" s="6"/>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A168" s="1" t="s">
+      <c r="C168" s="6"/>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" s="1" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A169" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B169" s="7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B170" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B170" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B171" s="6"/>
+      <c r="B171" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B172" s="6" t="s">
+      <c r="B172" s="6"/>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B173" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C172" s="6" t="s">
+      <c r="C173" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D172" t="s">
+      <c r="D173" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
-        <v>1</v>
-      </c>
-      <c r="B173" s="6">
-        <v>0.7</v>
-      </c>
-      <c r="C173" s="6">
-        <v>0.08</v>
-      </c>
-      <c r="D173" t="s">
-        <v>5</v>
-      </c>
-      <c r="E173" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>97</v>
+        <v>1</v>
       </c>
       <c r="B174" s="6">
-        <v>2</v>
-      </c>
-      <c r="C174" s="6" t="s">
-        <v>100</v>
+        <v>0.7</v>
+      </c>
+      <c r="C174" s="6">
+        <v>0.08</v>
       </c>
       <c r="D174" t="s">
-        <v>98</v>
+        <v>5</v>
       </c>
       <c r="E174" t="s">
-        <v>99</v>
+        <v>9</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
+        <v>97</v>
+      </c>
+      <c r="B175" s="6">
         <v>2</v>
       </c>
-      <c r="B175" s="6">
-        <v>0.99</v>
-      </c>
-      <c r="C175" s="6">
-        <v>0.99</v>
+      <c r="C175" s="6" t="s">
+        <v>100</v>
       </c>
       <c r="D175" t="s">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="E175" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B176" s="6">
-        <v>1E-3</v>
+        <v>0.99</v>
       </c>
       <c r="C176" s="6">
-        <v>1E-3</v>
+        <v>0.99</v>
       </c>
       <c r="D176" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E176" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>89</v>
+        <v>3</v>
       </c>
       <c r="B177" s="6">
-        <v>0</v>
-      </c>
-      <c r="C177" s="6"/>
+        <v>1E-3</v>
+      </c>
+      <c r="C177" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="D177" t="s">
+        <v>6</v>
+      </c>
+      <c r="E177" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B178" s="6">
-        <v>1</v>
-      </c>
-      <c r="C178" s="6">
-        <v>1</v>
-      </c>
-      <c r="D178" t="s">
-        <v>87</v>
-      </c>
-      <c r="E178" t="s">
-        <v>88</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C178" s="6"/>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="B179" s="6">
-        <v>300</v>
-      </c>
-      <c r="C179" s="6" t="s">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C179" s="6">
+        <v>1</v>
+      </c>
+      <c r="D179" t="s">
+        <v>87</v>
       </c>
       <c r="E179" t="s">
-        <v>0</v>
+        <v>88</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
+        <v>102</v>
+      </c>
+      <c r="B180" s="6">
+        <v>300</v>
+      </c>
+      <c r="C180" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E180" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
         <v>48</v>
       </c>
-      <c r="B180" s="6">
+      <c r="B181" s="6">
         <v>0.05</v>
       </c>
-      <c r="C180" s="6"/>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B181" s="6"/>
       <c r="C181" s="6"/>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>103</v>
-      </c>
-      <c r="B182" s="6">
-        <v>0.02</v>
-      </c>
+      <c r="B182" s="6"/>
       <c r="C182" s="6"/>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="B183" s="6">
-        <v>3600</v>
-      </c>
-      <c r="C183" s="6">
-        <v>3600</v>
-      </c>
-      <c r="D183" t="s">
-        <v>7</v>
-      </c>
-      <c r="E183" t="s">
-        <v>13</v>
-      </c>
+        <v>0.02</v>
+      </c>
+      <c r="C183" s="6"/>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B184" s="6">
-        <v>50000</v>
+        <v>3600</v>
       </c>
       <c r="C184" s="6">
-        <v>50000</v>
+        <v>3600</v>
       </c>
       <c r="D184" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E184" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
+        <v>65</v>
+      </c>
+      <c r="B185" s="6">
+        <v>50000</v>
+      </c>
+      <c r="C185" s="6">
+        <v>50000</v>
+      </c>
+      <c r="D185" t="s">
+        <v>8</v>
+      </c>
+      <c r="E185" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
         <v>43</v>
       </c>
-      <c r="B185" s="6"/>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B186" s="6"/>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B187" s="6"/>
-      <c r="C187" s="6"/>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A188" s="1" t="s">
+      <c r="B188" s="6"/>
+      <c r="C188" s="6"/>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A189" s="2" t="s">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B189" s="7" t="s">
+      <c r="B190" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C189" s="6"/>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B190" s="6"/>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A192" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B192" t="s">
-        <v>16</v>
-      </c>
+      <c r="C190" s="6"/>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B191" s="6"/>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B193" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B193">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B195" t="s">
+      <c r="B194">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B196" t="s">
         <v>17</v>
       </c>
-      <c r="C195" t="s">
+      <c r="C196" t="s">
         <v>18</v>
       </c>
-      <c r="D195" t="s">
+      <c r="D196" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A196" t="s">
-        <v>1</v>
-      </c>
-      <c r="B196">
-        <v>0.15</v>
-      </c>
-      <c r="C196">
-        <v>0.15</v>
-      </c>
-      <c r="D196" t="s">
-        <v>5</v>
-      </c>
-      <c r="E196" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B197">
-        <v>0.99</v>
+        <v>0.15</v>
       </c>
       <c r="C197">
-        <v>0.99</v>
+        <v>0.15</v>
       </c>
       <c r="D197" t="s">
         <v>5</v>
       </c>
       <c r="E197" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
+        <v>2</v>
+      </c>
+      <c r="B198">
+        <v>0.99</v>
+      </c>
+      <c r="C198">
+        <v>0.99</v>
+      </c>
+      <c r="D198" t="s">
+        <v>5</v>
+      </c>
+      <c r="E198" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
         <v>3</v>
       </c>
-      <c r="B198">
+      <c r="B199">
         <v>1E-3</v>
       </c>
-      <c r="C198">
+      <c r="C199">
         <v>1E-3</v>
       </c>
-      <c r="D198" t="s">
+      <c r="D199" t="s">
         <v>6</v>
       </c>
-      <c r="E198" t="s">
+      <c r="E199" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
-        <v>86</v>
-      </c>
-      <c r="B200">
-        <v>1</v>
-      </c>
-      <c r="C200">
-        <v>1</v>
-      </c>
-      <c r="D200" t="s">
-        <v>87</v>
-      </c>
-      <c r="E200" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>0</v>
-      </c>
-      <c r="B201" t="s">
-        <v>0</v>
-      </c>
-      <c r="C201" t="s">
-        <v>0</v>
+        <v>86</v>
+      </c>
+      <c r="B201">
+        <v>1</v>
+      </c>
+      <c r="C201">
+        <v>1</v>
+      </c>
+      <c r="D201" t="s">
+        <v>87</v>
       </c>
       <c r="E201" t="s">
-        <v>0</v>
+        <v>88</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>64</v>
-      </c>
-      <c r="B202">
-        <v>3600</v>
-      </c>
-      <c r="C202">
-        <v>3600</v>
-      </c>
-      <c r="D202" t="s">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="B202" t="s">
+        <v>0</v>
+      </c>
+      <c r="C202" t="s">
+        <v>0</v>
       </c>
       <c r="E202" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
+        <v>64</v>
+      </c>
+      <c r="B203">
+        <v>3600</v>
+      </c>
+      <c r="C203">
+        <v>3600</v>
+      </c>
+      <c r="D203" t="s">
+        <v>7</v>
+      </c>
+      <c r="E203" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
         <v>65</v>
       </c>
-      <c r="B203">
+      <c r="B204">
         <v>50000</v>
       </c>
-      <c r="C203">
+      <c r="C204">
         <v>50000</v>
       </c>
-      <c r="D203" t="s">
+      <c r="D204" t="s">
         <v>8</v>
       </c>
-      <c r="E203" t="s">
+      <c r="E204" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
         <v>83</v>
       </c>
-      <c r="B205">
+      <c r="B206">
         <v>3</v>
       </c>
-      <c r="E205" t="s">
+      <c r="E206" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
-        <v>93</v>
-      </c>
-      <c r="B207" s="9">
-        <v>1.0000000000000001E-5</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>94</v>
-      </c>
-      <c r="B208">
-        <v>0.1</v>
+        <v>93</v>
+      </c>
+      <c r="B208" s="9">
+        <v>1.0000000000000001E-5</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B209">
         <v>0.1</v>
@@ -2736,210 +2752,210 @@
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B210">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
+        <v>96</v>
+      </c>
+      <c r="B211">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A213" s="2"/>
-    </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A214" s="1" t="s">
+      <c r="A214" s="2"/>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A215" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A215" s="2" t="s">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A216" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B215" s="7" t="s">
+      <c r="B216" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C215" s="6"/>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B216" s="6"/>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A218" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B218" t="s">
-        <v>16</v>
-      </c>
+      <c r="C216" s="6"/>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B217" s="6"/>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B219" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B219">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B221" t="s">
+      <c r="B220">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B222" t="s">
         <v>17</v>
       </c>
-      <c r="C221" t="s">
+      <c r="C222" t="s">
         <v>18</v>
       </c>
-      <c r="D221" t="s">
+      <c r="D222" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A222" t="s">
-        <v>1</v>
-      </c>
-      <c r="B222">
-        <v>0.15</v>
-      </c>
-      <c r="C222">
-        <v>0.15</v>
-      </c>
-      <c r="D222" t="s">
-        <v>5</v>
-      </c>
-      <c r="E222" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B223">
-        <v>0.99</v>
+        <v>0.15</v>
       </c>
       <c r="C223">
-        <v>0.99</v>
+        <v>0.15</v>
       </c>
       <c r="D223" t="s">
         <v>5</v>
       </c>
       <c r="E223" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
+        <v>2</v>
+      </c>
+      <c r="B224">
+        <v>0.99</v>
+      </c>
+      <c r="C224">
+        <v>0.99</v>
+      </c>
+      <c r="D224" t="s">
+        <v>5</v>
+      </c>
+      <c r="E224" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
         <v>3</v>
       </c>
-      <c r="B224">
+      <c r="B225">
         <v>1E-3</v>
       </c>
-      <c r="C224">
+      <c r="C225">
         <v>1E-3</v>
       </c>
-      <c r="D224" t="s">
+      <c r="D225" t="s">
         <v>6</v>
       </c>
-      <c r="E224" t="s">
+      <c r="E225" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A226" t="s">
-        <v>86</v>
-      </c>
-      <c r="B226">
-        <v>1</v>
-      </c>
-      <c r="C226">
-        <v>1</v>
-      </c>
-      <c r="D226" t="s">
-        <v>87</v>
-      </c>
-      <c r="E226" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>0</v>
-      </c>
-      <c r="B227" t="s">
-        <v>0</v>
-      </c>
-      <c r="C227" t="s">
-        <v>0</v>
+        <v>86</v>
+      </c>
+      <c r="B227">
+        <v>1</v>
+      </c>
+      <c r="C227">
+        <v>1</v>
+      </c>
+      <c r="D227" t="s">
+        <v>87</v>
       </c>
       <c r="E227" t="s">
-        <v>0</v>
+        <v>88</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>64</v>
-      </c>
-      <c r="B228">
-        <v>3600</v>
-      </c>
-      <c r="C228">
-        <v>3600</v>
-      </c>
-      <c r="D228" t="s">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="B228" t="s">
+        <v>0</v>
+      </c>
+      <c r="C228" t="s">
+        <v>0</v>
       </c>
       <c r="E228" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
+        <v>64</v>
+      </c>
+      <c r="B229">
+        <v>3600</v>
+      </c>
+      <c r="C229">
+        <v>3600</v>
+      </c>
+      <c r="D229" t="s">
+        <v>7</v>
+      </c>
+      <c r="E229" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
         <v>65</v>
       </c>
-      <c r="B229">
+      <c r="B230">
         <v>50000</v>
       </c>
-      <c r="C229">
+      <c r="C230">
         <v>50000</v>
       </c>
-      <c r="D229" t="s">
+      <c r="D230" t="s">
         <v>8</v>
       </c>
-      <c r="E229" t="s">
+      <c r="E230" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A231" t="s">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
         <v>83</v>
       </c>
-      <c r="B231">
+      <c r="B232">
         <v>3</v>
       </c>
-      <c r="E231" t="s">
+      <c r="E232" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A233" t="s">
-        <v>93</v>
-      </c>
-      <c r="B233" s="9">
-        <v>1.0000000000000001E-5</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>94</v>
-      </c>
-      <c r="B234">
-        <v>0.1</v>
+        <v>93</v>
+      </c>
+      <c r="B234" s="9">
+        <v>1.0000000000000001E-5</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B235">
         <v>0.1</v>
@@ -2947,23 +2963,27 @@
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B236">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
+        <v>96</v>
+      </c>
+      <c r="B237">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A239" s="2"/>
-    </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B240" s="6"/>
-      <c r="C240" s="6"/>
+      <c r="A240" s="2"/>
     </row>
     <row r="241" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B241" s="6"/>
@@ -3033,19 +3053,18 @@
       <c r="B257" s="6"/>
       <c r="C257" s="6"/>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B260" s="6"/>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B258" s="6"/>
+      <c r="C258" s="6"/>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B261" s="6"/>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A262" s="1"/>
+      <c r="B262" s="6"/>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A263" s="2"/>
-      <c r="B263" s="7"/>
-      <c r="C263" s="6"/>
+      <c r="A263" s="1"/>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" s="2"/>
@@ -3053,7 +3072,8 @@
       <c r="C264" s="6"/>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B265" s="6"/>
+      <c r="A265" s="2"/>
+      <c r="B265" s="7"/>
       <c r="C265" s="6"/>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
@@ -3105,7 +3125,11 @@
       <c r="C277" s="6"/>
     </row>
     <row r="278" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B278" s="6"/>
       <c r="C278" s="6"/>
+    </row>
+    <row r="279" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C279" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
CHANGED: IA_CLASS changed to LATERAL_IA_CLASS, LATERAL_IA_xD changed to LATERAL_xD. Runfiles and parameter files updated.
</commit_message>
<xml_diff>
--- a/results/Finse_4432/Finse_4432.xlsx
+++ b/results/Finse_4432/Finse_4432.xlsx
@@ -491,9 +491,6 @@
     <t>GROUND_CLASS</t>
   </si>
   <si>
-    <t>IA_CLASS</t>
-  </si>
-  <si>
     <t>reservoir_elevation</t>
   </si>
   <si>
@@ -521,10 +518,13 @@
     <t>LATERAL_CLASS</t>
   </si>
   <si>
-    <t>LATERAL_IA_1D</t>
-  </si>
-  <si>
-    <t>LATERAL_IA_3D</t>
+    <t>LATERAL_IA_CLASS</t>
+  </si>
+  <si>
+    <t>LATERAL_1D</t>
+  </si>
+  <si>
+    <t>LATERAL_3D</t>
   </si>
 </sst>
 </file>
@@ -869,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G272"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A222" workbookViewId="0">
-      <selection activeCell="B237" sqref="B237"/>
+    <sheetView tabSelected="1" topLeftCell="A236" workbookViewId="0">
+      <selection activeCell="A261" sqref="A261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1048,7 +1048,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B15">
         <v>0.25</v>
@@ -3009,7 +3009,7 @@
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="B237" s="2" t="s">
         <v>15</v>
@@ -3042,7 +3042,7 @@
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B241" s="6">
         <v>20</v>
@@ -3051,31 +3051,31 @@
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B242" s="6">
         <v>0.5</v>
       </c>
       <c r="C242" s="6"/>
       <c r="E242" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B243" s="6">
         <v>0.03</v>
       </c>
       <c r="C243" s="6"/>
       <c r="E243" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B244" s="6">
         <v>3</v>
@@ -3084,7 +3084,7 @@
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B245" s="6">
         <v>1</v>
@@ -3113,7 +3113,7 @@
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B250" s="2" t="s">
         <v>15</v>
@@ -3146,7 +3146,7 @@
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B254">
         <v>0.25</v>
@@ -3175,7 +3175,7 @@
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B259" s="2" t="s">
         <v>15</v>
@@ -3208,7 +3208,7 @@
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B263">
         <v>0.05</v>

</xml_diff>